<commit_message>
fix: excel date format
</commit_message>
<xml_diff>
--- a/src/common/importData/transportsDataCleaned.xlsx
+++ b/src/common/importData/transportsDataCleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim.naish\Desktop\CMMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B37D1D-CEAE-445C-8CFF-B48578942BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328D8C06-A2C2-44A1-A039-EFDF41C281E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{40E9A6BE-C268-4259-B0FD-00503ABF1BC9}"/>
   </bookViews>
@@ -605,6 +605,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -794,46 +797,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFDB0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFED7D31"/>
-      </font>
-    </dxf>
+  <dxfs count="95">
     <dxf>
       <font>
         <b/>
@@ -1005,89 +979,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFE68600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFD40000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFE68600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFD40000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFE68600"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFD40000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2351,8 +2242,8 @@
   <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6366,462 +6257,462 @@
     <protectedRange sqref="G2:G110" name="Update_1"/>
   </protectedRanges>
   <conditionalFormatting sqref="A106:A108 H11:H55 D54:D68 C11:F55 A96 C98:H98 C100:H100 C102:H110 H57:H88 C57:F88 G6:G88 C89:H94 C96:H96">
-    <cfRule type="expression" dxfId="104" priority="137">
+    <cfRule type="expression" dxfId="94" priority="137">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106:A108 H11:H55 D54:D68 C11:F55 A96 C98:H98 C100:H100 C102:H110 H57:H88 C57:F88 G6:G88 C89:H94 C96:H96">
-    <cfRule type="expression" dxfId="103" priority="136">
+    <cfRule type="expression" dxfId="93" priority="136">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106:A108 A96 C98:H98 C100:H100 C102:H110 C6:H94 C96:H96 C5:F5 H5">
-    <cfRule type="expression" dxfId="102" priority="135">
+    <cfRule type="expression" dxfId="92" priority="135">
       <formula>SEARCH("disposal", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C9">
-    <cfRule type="expression" dxfId="101" priority="132">
+    <cfRule type="expression" dxfId="91" priority="132">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C9">
-    <cfRule type="expression" dxfId="100" priority="131">
+    <cfRule type="expression" dxfId="90" priority="131">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="99" priority="130">
+    <cfRule type="expression" dxfId="89" priority="130">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="98" priority="129">
+    <cfRule type="expression" dxfId="88" priority="129">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="97" priority="128">
+    <cfRule type="expression" dxfId="87" priority="128">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="96" priority="127">
+    <cfRule type="expression" dxfId="86" priority="127">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="95" priority="126">
+    <cfRule type="expression" dxfId="85" priority="126">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="94" priority="125">
+    <cfRule type="expression" dxfId="84" priority="125">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="expression" dxfId="93" priority="121">
+    <cfRule type="expression" dxfId="83" priority="121">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="expression" dxfId="92" priority="120">
+    <cfRule type="expression" dxfId="82" priority="120">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="91" priority="119">
+    <cfRule type="expression" dxfId="81" priority="119">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="90" priority="118">
+    <cfRule type="expression" dxfId="80" priority="118">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="89" priority="117">
+    <cfRule type="expression" dxfId="79" priority="117">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="88" priority="116">
+    <cfRule type="expression" dxfId="78" priority="116">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="87" priority="115">
+    <cfRule type="expression" dxfId="77" priority="115">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="86" priority="114">
+    <cfRule type="expression" dxfId="76" priority="114">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E9">
-    <cfRule type="expression" dxfId="85" priority="110">
+    <cfRule type="expression" dxfId="75" priority="110">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E9">
-    <cfRule type="expression" dxfId="84" priority="109">
+    <cfRule type="expression" dxfId="74" priority="109">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="83" priority="108">
+    <cfRule type="expression" dxfId="73" priority="108">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="82" priority="107">
+    <cfRule type="expression" dxfId="72" priority="107">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="81" priority="106">
+    <cfRule type="expression" dxfId="71" priority="106">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="80" priority="105">
+    <cfRule type="expression" dxfId="70" priority="105">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="79" priority="104">
+    <cfRule type="expression" dxfId="69" priority="104">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="78" priority="103">
+    <cfRule type="expression" dxfId="68" priority="103">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F9">
-    <cfRule type="expression" dxfId="77" priority="99">
+    <cfRule type="expression" dxfId="67" priority="99">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F9">
-    <cfRule type="expression" dxfId="76" priority="98">
+    <cfRule type="expression" dxfId="66" priority="98">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="75" priority="97">
+    <cfRule type="expression" dxfId="65" priority="97">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="74" priority="96">
+    <cfRule type="expression" dxfId="64" priority="96">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="73" priority="95">
+    <cfRule type="expression" dxfId="63" priority="95">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="72" priority="94">
+    <cfRule type="expression" dxfId="62" priority="94">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="expression" dxfId="69" priority="86">
+    <cfRule type="expression" dxfId="61" priority="86">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="expression" dxfId="68" priority="85">
+    <cfRule type="expression" dxfId="60" priority="85">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="67" priority="84">
+    <cfRule type="expression" dxfId="59" priority="84">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="66" priority="83">
+    <cfRule type="expression" dxfId="58" priority="83">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="63" priority="79">
+    <cfRule type="expression" dxfId="57" priority="79">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="62" priority="78">
+    <cfRule type="expression" dxfId="56" priority="78">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="expression" dxfId="61" priority="77">
+    <cfRule type="expression" dxfId="55" priority="77">
       <formula>SEARCH("breakdown", $K58)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="expression" dxfId="60" priority="76">
+    <cfRule type="expression" dxfId="54" priority="76">
       <formula>SEARCH("issues", $K58)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="59" priority="75">
+    <cfRule type="expression" dxfId="53" priority="75">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="58" priority="74">
+    <cfRule type="expression" dxfId="52" priority="74">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="expression" dxfId="57" priority="73">
+    <cfRule type="expression" dxfId="51" priority="73">
       <formula>SEARCH("breakdown", $K57)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="expression" dxfId="56" priority="72">
+    <cfRule type="expression" dxfId="50" priority="72">
       <formula>SEARCH("issues", $K57)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H9">
-    <cfRule type="expression" dxfId="55" priority="69">
+    <cfRule type="expression" dxfId="49" priority="69">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H9">
-    <cfRule type="expression" dxfId="54" priority="68">
+    <cfRule type="expression" dxfId="48" priority="68">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="expression" dxfId="53" priority="67">
+    <cfRule type="expression" dxfId="47" priority="67">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="expression" dxfId="52" priority="66">
+    <cfRule type="expression" dxfId="46" priority="66">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="51" priority="65">
+    <cfRule type="expression" dxfId="45" priority="65">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="50" priority="64">
+    <cfRule type="expression" dxfId="44" priority="64">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="49" priority="63">
+    <cfRule type="expression" dxfId="43" priority="63">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="48" priority="62">
+    <cfRule type="expression" dxfId="42" priority="62">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="expression" dxfId="47" priority="57">
+    <cfRule type="expression" dxfId="41" priority="57">
       <formula>SEARCH("breakdown", $K69)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="expression" dxfId="46" priority="56">
+    <cfRule type="expression" dxfId="40" priority="56">
       <formula>SEARCH("issues", $K69)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="45" priority="55">
+    <cfRule type="expression" dxfId="39" priority="55">
       <formula>SEARCH("breakdown", $K70)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="44" priority="54">
+    <cfRule type="expression" dxfId="38" priority="54">
       <formula>SEARCH("issues", $K70)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="43" priority="53">
+    <cfRule type="expression" dxfId="37" priority="53">
       <formula>SEARCH("breakdown", $K74)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="42" priority="52">
+    <cfRule type="expression" dxfId="36" priority="52">
       <formula>SEARCH("issues", $K74)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="41" priority="51">
+    <cfRule type="expression" dxfId="35" priority="51">
       <formula>SEARCH("breakdown", $K75)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="40" priority="50">
+    <cfRule type="expression" dxfId="34" priority="50">
       <formula>SEARCH("issues", $K75)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="39" priority="49">
+    <cfRule type="expression" dxfId="33" priority="49">
       <formula>SEARCH("breakdown", $K76)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="38" priority="48">
+    <cfRule type="expression" dxfId="32" priority="48">
       <formula>SEARCH("issues", $K76)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="31" priority="47">
       <formula>SEARCH("breakdown", $K77)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="36" priority="46">
+    <cfRule type="expression" dxfId="30" priority="46">
       <formula>SEARCH("issues", $K77)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="35" priority="45">
+    <cfRule type="expression" dxfId="29" priority="45">
       <formula>SEARCH("breakdown", $K7)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="28" priority="44">
       <formula>SEARCH("issues", $K7)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="33" priority="43">
+    <cfRule type="expression" dxfId="27" priority="43">
       <formula>SEARCH("breakdown", $K11)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="32" priority="42">
+    <cfRule type="expression" dxfId="26" priority="42">
       <formula>SEARCH("issues", $K11)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="31" priority="41">
+    <cfRule type="expression" dxfId="25" priority="41">
       <formula>SEARCH("breakdown", $K104)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="30" priority="40">
+    <cfRule type="expression" dxfId="24" priority="40">
       <formula>SEARCH("issues", $K104)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="23" priority="39">
       <formula>SEARCH("breakdown", $K105)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="28" priority="38">
+    <cfRule type="expression" dxfId="22" priority="38">
       <formula>SEARCH("issues", $K105)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="27" priority="37">
+    <cfRule type="expression" dxfId="21" priority="37">
       <formula>SEARCH("breakdown", $K106)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="26" priority="36">
+    <cfRule type="expression" dxfId="20" priority="36">
       <formula>SEARCH("issues", $K106)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="25" priority="35">
+    <cfRule type="expression" dxfId="19" priority="35">
       <formula>SEARCH("breakdown", $K107)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="24" priority="34">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>SEARCH("issues", $K107)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>SEARCH("breakdown", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>SEARCH("issues", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>SEARCH("disposal", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>SEARCH("breakdown", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>SEARCH("issues", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>SEARCH("disposal", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="11" priority="15">
       <formula>SEARCH("breakdown", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>SEARCH("issues", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>SEARCH("disposal", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>SEARCH("breakdown", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>SEARCH("issues", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>SEARCH("disposal", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>SEARCH("major issues", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>SEARCH("disposal", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>SEARCH("breakdown", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat (entity): all code rewritten
</commit_message>
<xml_diff>
--- a/src/common/importData/transportsDataCleaned.xlsx
+++ b/src/common/importData/transportsDataCleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibrahim.naish\Desktop\cmms-api\cmms-api\src\common\importData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026DD730-2897-487D-883E-AD9F2A0404D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539E62D4-6C90-49B1-8CA2-9171671E0BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{40E9A6BE-C268-4259-B0FD-00503ABF1BC9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="185">
   <si>
     <t>SUZUKI</t>
   </si>
@@ -319,9 +319,6 @@
     <t xml:space="preserve">YUTONG </t>
   </si>
   <si>
-    <t xml:space="preserve">Double Decker </t>
-  </si>
-  <si>
     <t>C1220</t>
   </si>
   <si>
@@ -400,9 +397,6 @@
     <t>C2747</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorry </t>
-  </si>
-  <si>
     <t>CDD</t>
   </si>
   <si>
@@ -532,9 +526,6 @@
     <t>T1110</t>
   </si>
   <si>
-    <t xml:space="preserve">Forklift </t>
-  </si>
-  <si>
     <t>Aila</t>
   </si>
   <si>
@@ -599,6 +590,9 @@
   </si>
   <si>
     <t>L. Maavah</t>
+  </si>
+  <si>
+    <t>uniqueType</t>
   </si>
 </sst>
 </file>
@@ -807,35 +801,373 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFDB0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFED7D31"/>
-      </font>
+  <dxfs count="123">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFE68600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFD40000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2239,11 +2571,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F548B326-95FE-4056-A630-56C04AC97D8E}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2261,52 +2593,56 @@
     <col min="11" max="11" width="17.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.54296875" customWidth="1"/>
     <col min="13" max="13" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="E1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="J1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N1" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>0</v>
@@ -2321,7 +2657,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>4</v>
@@ -2336,15 +2672,18 @@
         <v>4035</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>0</v>
@@ -2359,7 +2698,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>4</v>
@@ -2374,15 +2713,16 @@
         <v>488</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>0</v>
@@ -2391,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>4</v>
@@ -2412,13 +2752,14 @@
         <v>1590</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2430,13 +2771,13 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>12</v>
@@ -2454,8 +2795,11 @@
       <c r="M5" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
@@ -2467,13 +2811,13 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>12</v>
@@ -2491,8 +2835,11 @@
       <c r="M6" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N6" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>19</v>
       </c>
@@ -2507,10 +2854,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>12</v>
@@ -2528,8 +2875,9 @@
       <c r="M7" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
@@ -2541,13 +2889,13 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>12</v>
@@ -2565,8 +2913,9 @@
       <c r="M8" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
@@ -2578,13 +2927,13 @@
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>12</v>
@@ -2602,8 +2951,9 @@
       <c r="M9" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
@@ -2623,7 +2973,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>27</v>
@@ -2641,8 +2991,11 @@
       <c r="M10" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N10" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
@@ -2662,7 +3015,7 @@
         <v>26</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>27</v>
@@ -2680,8 +3033,9 @@
       <c r="M11" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
@@ -2699,7 +3053,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>27</v>
@@ -2717,8 +3071,9 @@
       <c r="M12" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
@@ -2730,13 +3085,13 @@
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>27</v>
@@ -2754,8 +3109,9 @@
       <c r="M13" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
@@ -2772,7 +3128,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>4</v>
@@ -2790,8 +3146,11 @@
       <c r="M14" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N14" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>36</v>
       </c>
@@ -2808,7 +3167,7 @@
         <v>37</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>4</v>
@@ -2826,8 +3185,9 @@
       <c r="M15" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>38</v>
       </c>
@@ -2844,7 +3204,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>4</v>
@@ -2862,8 +3222,9 @@
       <c r="M16" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N16" s="12"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>39</v>
       </c>
@@ -2880,7 +3241,7 @@
         <v>40</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>4</v>
@@ -2898,8 +3259,9 @@
       <c r="M17" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>41</v>
       </c>
@@ -2910,13 +3272,13 @@
         <v>34</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -2934,8 +3296,9 @@
       <c r="M18" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>43</v>
       </c>
@@ -2946,13 +3309,13 @@
         <v>44</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
@@ -2970,8 +3333,9 @@
       <c r="M19" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>46</v>
       </c>
@@ -2988,7 +3352,7 @@
         <v>45</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>4</v>
@@ -3006,8 +3370,9 @@
       <c r="M20" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>47</v>
       </c>
@@ -3018,13 +3383,13 @@
         <v>44</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>4</v>
@@ -3042,8 +3407,9 @@
       <c r="M21" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>48</v>
       </c>
@@ -3054,13 +3420,13 @@
         <v>44</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>4</v>
@@ -3078,8 +3444,9 @@
       <c r="M22" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>49</v>
       </c>
@@ -3096,7 +3463,7 @@
         <v>42</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>4</v>
@@ -3114,8 +3481,9 @@
       <c r="M23" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N23" s="12"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>50</v>
       </c>
@@ -3132,7 +3500,7 @@
         <v>45</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>4</v>
@@ -3150,8 +3518,9 @@
       <c r="M24" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N24" s="12"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>51</v>
       </c>
@@ -3168,7 +3537,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>4</v>
@@ -3186,8 +3555,9 @@
       <c r="M25" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>52</v>
       </c>
@@ -3198,13 +3568,13 @@
         <v>44</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>4</v>
@@ -3222,8 +3592,9 @@
       <c r="M26" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>53</v>
       </c>
@@ -3243,7 +3614,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>27</v>
@@ -3261,8 +3632,9 @@
       <c r="M27" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N27" s="12"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>54</v>
       </c>
@@ -3282,7 +3654,7 @@
         <v>26</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>27</v>
@@ -3300,8 +3672,9 @@
       <c r="M28" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
         <v>55</v>
       </c>
@@ -3312,13 +3685,13 @@
         <v>57</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>27</v>
@@ -3336,8 +3709,9 @@
       <c r="M29" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N29" s="12"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>58</v>
       </c>
@@ -3354,7 +3728,7 @@
         <v>26</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>27</v>
@@ -3372,8 +3746,9 @@
       <c r="M30" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>60</v>
       </c>
@@ -3390,7 +3765,7 @@
         <v>26</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>27</v>
@@ -3408,8 +3783,9 @@
       <c r="M31" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>61</v>
       </c>
@@ -3426,7 +3802,7 @@
         <v>26</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>27</v>
@@ -3444,8 +3820,9 @@
       <c r="M32" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>62</v>
       </c>
@@ -3462,7 +3839,7 @@
         <v>26</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>27</v>
@@ -3480,8 +3857,9 @@
       <c r="M33" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N33" s="12"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>63</v>
       </c>
@@ -3498,7 +3876,7 @@
         <v>26</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>27</v>
@@ -3516,8 +3894,9 @@
       <c r="M34" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N34" s="12"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>64</v>
       </c>
@@ -3534,7 +3913,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>27</v>
@@ -3552,8 +3931,9 @@
       <c r="M35" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N35" s="12"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>65</v>
       </c>
@@ -3564,13 +3944,13 @@
         <v>59</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>27</v>
@@ -3588,8 +3968,9 @@
       <c r="M36" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
         <v>66</v>
       </c>
@@ -3600,13 +3981,13 @@
         <v>57</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>27</v>
@@ -3624,8 +4005,9 @@
       <c r="M37" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N37" s="12"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
         <v>67</v>
       </c>
@@ -3636,13 +4018,13 @@
         <v>68</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>27</v>
@@ -3660,8 +4042,11 @@
       <c r="M38" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N38" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>70</v>
       </c>
@@ -3678,7 +4063,7 @@
         <v>26</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>27</v>
@@ -3696,8 +4081,9 @@
       <c r="M39" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N39" s="12"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
         <v>71</v>
       </c>
@@ -3714,7 +4100,7 @@
         <v>26</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>27</v>
@@ -3732,8 +4118,9 @@
       <c r="M40" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>72</v>
       </c>
@@ -3750,7 +4137,7 @@
         <v>26</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>27</v>
@@ -3768,8 +4155,9 @@
       <c r="M41" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>73</v>
       </c>
@@ -3786,7 +4174,7 @@
         <v>26</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>27</v>
@@ -3804,8 +4192,9 @@
       <c r="M42" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N42" s="12"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>74</v>
       </c>
@@ -3816,13 +4205,13 @@
         <v>57</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>27</v>
@@ -3840,8 +4229,9 @@
       <c r="M43" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>75</v>
       </c>
@@ -3858,7 +4248,7 @@
         <v>26</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>27</v>
@@ -3876,8 +4266,9 @@
       <c r="M44" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>76</v>
       </c>
@@ -3894,7 +4285,7 @@
         <v>26</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H45" s="12" t="s">
         <v>27</v>
@@ -3912,8 +4303,9 @@
       <c r="M45" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N45" s="12"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>77</v>
       </c>
@@ -3930,7 +4322,7 @@
         <v>26</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>27</v>
@@ -3948,8 +4340,9 @@
       <c r="M46" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>78</v>
       </c>
@@ -3966,7 +4359,7 @@
         <v>26</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>27</v>
@@ -3984,8 +4377,9 @@
       <c r="M47" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>79</v>
       </c>
@@ -4002,7 +4396,7 @@
         <v>26</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H48" s="12" t="s">
         <v>27</v>
@@ -4020,8 +4414,9 @@
       <c r="M48" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N48" s="12"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>80</v>
       </c>
@@ -4038,7 +4433,7 @@
         <v>26</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>27</v>
@@ -4056,8 +4451,9 @@
       <c r="M49" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N49" s="12"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>81</v>
       </c>
@@ -4068,13 +4464,13 @@
         <v>68</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>27</v>
@@ -4092,8 +4488,9 @@
       <c r="M50" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N50" s="12"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>82</v>
       </c>
@@ -4113,7 +4510,7 @@
         <v>26</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>27</v>
@@ -4131,8 +4528,11 @@
       <c r="M51" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N51" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>86</v>
       </c>
@@ -4152,7 +4552,7 @@
         <v>26</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>27</v>
@@ -4170,8 +4570,9 @@
       <c r="M52" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N52" s="12"/>
+    </row>
+    <row r="53" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>88</v>
       </c>
@@ -4185,13 +4586,13 @@
         <v>89</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>90</v>
@@ -4209,8 +4610,9 @@
       <c r="M53" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N53" s="12"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>91</v>
       </c>
@@ -4224,13 +4626,13 @@
         <v>68</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>27</v>
@@ -4248,10 +4650,11 @@
       <c r="M54" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N54" s="12"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55" s="29">
         <v>44706</v>
@@ -4263,13 +4666,13 @@
         <v>68</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>27</v>
@@ -4287,10 +4690,11 @@
       <c r="M55" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N55" s="12"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="29">
         <v>44706</v>
@@ -4302,13 +4706,13 @@
         <v>68</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>27</v>
@@ -4326,10 +4730,11 @@
       <c r="M56" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N56" s="12"/>
+    </row>
+    <row r="57" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B57" s="29">
         <v>44706</v>
@@ -4341,13 +4746,13 @@
         <v>68</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>27</v>
@@ -4365,10 +4770,11 @@
       <c r="M57" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N57" s="12"/>
+    </row>
+    <row r="58" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" s="29">
         <v>44706</v>
@@ -4380,13 +4786,13 @@
         <v>68</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>27</v>
@@ -4404,10 +4810,11 @@
       <c r="M58" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N58" s="12"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="29">
         <v>44706</v>
@@ -4419,13 +4826,13 @@
         <v>68</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>27</v>
@@ -4443,10 +4850,11 @@
       <c r="M59" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N59" s="12"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B60" s="29">
         <v>44706</v>
@@ -4458,13 +4866,13 @@
         <v>68</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>27</v>
@@ -4482,10 +4890,11 @@
       <c r="M60" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N60" s="12"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B61" s="29">
         <v>44706</v>
@@ -4497,13 +4906,13 @@
         <v>68</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>27</v>
@@ -4521,10 +4930,11 @@
       <c r="M61" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N61" s="12"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="29">
         <v>44706</v>
@@ -4536,13 +4946,13 @@
         <v>68</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H62" s="12" t="s">
         <v>27</v>
@@ -4560,10 +4970,11 @@
       <c r="M62" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N62" s="12"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63" s="29">
         <v>44706</v>
@@ -4575,13 +4986,13 @@
         <v>68</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H63" s="12" t="s">
         <v>27</v>
@@ -4599,10 +5010,11 @@
       <c r="M63" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N63" s="12"/>
+    </row>
+    <row r="64" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="29">
         <v>44706</v>
@@ -4614,13 +5026,13 @@
         <v>68</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>27</v>
@@ -4638,10 +5050,11 @@
       <c r="M64" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N64" s="12"/>
+    </row>
+    <row r="65" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" s="29">
         <v>44706</v>
@@ -4653,13 +5066,13 @@
         <v>68</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>27</v>
@@ -4677,10 +5090,11 @@
       <c r="M65" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N65" s="12"/>
+    </row>
+    <row r="66" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B66" s="29">
         <v>44706</v>
@@ -4692,13 +5106,13 @@
         <v>68</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>27</v>
@@ -4716,10 +5130,11 @@
       <c r="M66" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N66" s="12"/>
+    </row>
+    <row r="67" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B67" s="29">
         <v>44706</v>
@@ -4731,13 +5146,13 @@
         <v>68</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>27</v>
@@ -4755,10 +5170,11 @@
       <c r="M67" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N67" s="12"/>
+    </row>
+    <row r="68" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B68" s="29">
         <v>44706</v>
@@ -4770,13 +5186,13 @@
         <v>68</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G68" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H68" s="12" t="s">
         <v>27</v>
@@ -4794,10 +5210,11 @@
       <c r="M68" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N68" s="12"/>
+    </row>
+    <row r="69" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B69" s="29">
         <v>36923</v>
@@ -4810,10 +5227,10 @@
         <v>17</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H69" s="12" t="s">
         <v>12</v>
@@ -4831,10 +5248,11 @@
       <c r="M69" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N69" s="12"/>
+    </row>
+    <row r="70" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B70" s="29">
         <v>38046</v>
@@ -4847,10 +5265,10 @@
         <v>17</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>12</v>
@@ -4868,26 +5286,27 @@
       <c r="M70" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N70" s="12"/>
+    </row>
+    <row r="71" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="8">
@@ -4902,21 +5321,22 @@
       <c r="M71" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N71" s="12"/>
+    </row>
+    <row r="72" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H72" s="12" t="s">
         <v>90</v>
@@ -4934,26 +5354,29 @@
       <c r="M72" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N72" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H73" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I73" s="4"/>
       <c r="J73" s="8">
@@ -4968,26 +5391,27 @@
       <c r="M73" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N73" s="12"/>
+    </row>
+    <row r="74" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="8">
@@ -5002,10 +5426,11 @@
       <c r="M74" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N74" s="12"/>
+    </row>
+    <row r="75" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B75" s="29">
         <v>43258</v>
@@ -5018,13 +5443,13 @@
         <v>17</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="8">
@@ -5039,10 +5464,11 @@
       <c r="M75" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N75" s="12"/>
+    </row>
+    <row r="76" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B76" s="29">
         <v>36713</v>
@@ -5052,16 +5478,16 @@
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G76" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H76" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="8">
@@ -5076,26 +5502,27 @@
       <c r="M76" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N76" s="12"/>
+    </row>
+    <row r="77" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G77" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="8">
@@ -5110,26 +5537,27 @@
       <c r="M77" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N77" s="12"/>
+    </row>
+    <row r="78" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I78" s="4"/>
       <c r="J78" s="8">
@@ -5144,10 +5572,13 @@
       <c r="M78" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N78" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B79" s="29">
         <v>44294</v>
@@ -5157,13 +5588,13 @@
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H79" s="12" t="s">
         <v>12</v>
@@ -5181,24 +5612,25 @@
       <c r="M79" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N79" s="12"/>
+    </row>
+    <row r="80" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="12"/>
       <c r="E80" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H80" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I80" s="4"/>
       <c r="J80" s="8">
@@ -5213,21 +5645,24 @@
       <c r="M80" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N80" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="12"/>
       <c r="E81" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H81" s="12" t="s">
         <v>90</v>
@@ -5245,26 +5680,27 @@
       <c r="M81" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N81" s="12"/>
+    </row>
+    <row r="82" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G82" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I82" s="4"/>
       <c r="J82" s="8">
@@ -5279,26 +5715,27 @@
       <c r="M82" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N82" s="12"/>
+    </row>
+    <row r="83" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I83" s="4"/>
       <c r="J83" s="8">
@@ -5311,26 +5748,27 @@
       <c r="M83" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N83" s="12"/>
+    </row>
+    <row r="84" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="12" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G84" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I84" s="4"/>
       <c r="J84" s="8">
@@ -5345,10 +5783,11 @@
       <c r="M84" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N84" s="12"/>
+    </row>
+    <row r="85" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B85" s="29">
         <v>42725</v>
@@ -5357,16 +5796,16 @@
         <v>83</v>
       </c>
       <c r="D85" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H85" s="12" t="s">
         <v>27</v>
@@ -5382,21 +5821,22 @@
       <c r="M85" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N85" s="12"/>
+    </row>
+    <row r="86" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C86" s="13"/>
       <c r="D86" s="12"/>
       <c r="E86" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G86" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H86" s="22" t="s">
         <v>4</v>
@@ -5411,26 +5851,29 @@
         <v>8458</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M86" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N86" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C87" s="13"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G87" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H87" s="22" t="s">
         <v>4</v>
@@ -5445,26 +5888,27 @@
         <v>8458</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M87" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N87" s="12"/>
+    </row>
+    <row r="88" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="12"/>
       <c r="E88" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F88" s="23" t="s">
         <v>42</v>
       </c>
       <c r="G88" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H88" s="22" t="s">
         <v>4</v>
@@ -5479,15 +5923,18 @@
         <v>2798</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M88" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N88" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C89" s="13"/>
       <c r="D89" s="12"/>
@@ -5498,7 +5945,7 @@
         <v>42</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H89" s="22" t="s">
         <v>4</v>
@@ -5513,26 +5960,27 @@
         <v>2798</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M89" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N89" s="22"/>
+    </row>
+    <row r="90" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G90" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H90" s="12" t="s">
         <v>4</v>
@@ -5545,26 +5993,29 @@
         <v>4687</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M90" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N90" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C91" s="13"/>
       <c r="D91" s="12"/>
       <c r="E91" s="12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F91" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G91" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H91" s="12" t="s">
         <v>4</v>
@@ -5577,28 +6028,29 @@
         <v>2639</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M91" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N91" s="12"/>
+    </row>
+    <row r="92" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H92" s="12" t="s">
         <v>4</v>
@@ -5613,28 +6065,31 @@
         <v>0</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M92" s="27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N92" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="22" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F93" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H93" s="12" t="s">
         <v>4</v>
@@ -5649,28 +6104,29 @@
         <v>0</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M93" s="27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N93" s="22"/>
+    </row>
+    <row r="94" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G94" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H94" s="12" t="s">
         <v>4</v>
@@ -5685,28 +6141,31 @@
         <v>3904</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M94" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N94" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F95" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G95" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H95" s="12" t="s">
         <v>4</v>
@@ -5721,28 +6180,29 @@
         <v>3837</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M95" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N95" s="12"/>
+    </row>
+    <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G96" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H96" s="12" t="s">
         <v>4</v>
@@ -5757,28 +6217,29 @@
         <v>581</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M96" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N96" s="12"/>
+    </row>
+    <row r="97" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F97" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G97" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H97" s="12" t="s">
         <v>4</v>
@@ -5793,28 +6254,29 @@
         <v>581</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M97" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N97" s="12"/>
+    </row>
+    <row r="98" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D98" s="12"/>
       <c r="E98" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F98" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G98" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H98" s="12" t="s">
         <v>4</v>
@@ -5829,28 +6291,29 @@
         <v>3053</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M98" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N98" s="12"/>
+    </row>
+    <row r="99" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F99" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G99" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H99" s="12" t="s">
         <v>4</v>
@@ -5865,28 +6328,29 @@
         <v>3047</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M99" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N99" s="12"/>
+    </row>
+    <row r="100" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G100" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H100" s="12" t="s">
         <v>4</v>
@@ -5901,28 +6365,29 @@
         <v>3453</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M100" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N100" s="12"/>
+    </row>
+    <row r="101" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G101" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H101" s="12" t="s">
         <v>4</v>
@@ -5937,28 +6402,29 @@
         <v>3496</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M101" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N101" s="12"/>
+    </row>
+    <row r="102" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G102" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H102" s="12" t="s">
         <v>4</v>
@@ -5971,28 +6437,29 @@
         <v>0</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M102" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N102" s="12"/>
+    </row>
+    <row r="103" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G103" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H103" s="12" t="s">
         <v>4</v>
@@ -6005,15 +6472,16 @@
         <v>4149</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="M103" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N103" s="12"/>
+    </row>
+    <row r="104" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B104" s="29">
         <v>41436</v>
@@ -6022,7 +6490,7 @@
         <v>23</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E104" s="12" t="s">
         <v>35</v>
@@ -6031,7 +6499,7 @@
         <v>26</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H104" s="12" t="s">
         <v>27</v>
@@ -6049,10 +6517,11 @@
       <c r="M104" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N104" s="12"/>
+    </row>
+    <row r="105" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B105" s="29">
         <v>41436</v>
@@ -6061,7 +6530,7 @@
         <v>23</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E105" s="12" t="s">
         <v>35</v>
@@ -6070,7 +6539,7 @@
         <v>26</v>
       </c>
       <c r="G105" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H105" s="12" t="s">
         <v>27</v>
@@ -6088,10 +6557,11 @@
       <c r="M105" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N105" s="12"/>
+    </row>
+    <row r="106" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B106" s="29">
         <v>41436</v>
@@ -6100,7 +6570,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E106" s="12" t="s">
         <v>35</v>
@@ -6109,7 +6579,7 @@
         <v>26</v>
       </c>
       <c r="G106" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H106" s="12" t="s">
         <v>27</v>
@@ -6127,10 +6597,11 @@
       <c r="M106" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N106" s="12"/>
+    </row>
+    <row r="107" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B107" s="29">
         <v>41436</v>
@@ -6139,16 +6610,16 @@
         <v>23</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G107" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H107" s="12" t="s">
         <v>27</v>
@@ -6166,19 +6637,20 @@
       <c r="M107" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N107" s="12"/>
+    </row>
+    <row r="108" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="16"/>
       <c r="C108" s="13"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="F108" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G108" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H108" s="12" t="s">
         <v>12</v>
@@ -6194,22 +6666,23 @@
       <c r="M108" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N108" s="12"/>
+    </row>
+    <row r="109" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109" s="16"/>
       <c r="C109" s="13"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G109" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H109" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I109" s="4"/>
       <c r="J109" s="8">
@@ -6222,19 +6695,20 @@
       <c r="M109" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N109" s="12"/>
+    </row>
+    <row r="110" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A110" s="16"/>
       <c r="C110" s="13"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F110" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G110" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H110" s="12" t="s">
         <v>90</v>
@@ -6250,6 +6724,7 @@
       <c r="M110" s="15" t="s">
         <v>14</v>
       </c>
+      <c r="N110" s="12"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -6257,478 +6732,573 @@
     <protectedRange sqref="G2:G110" name="Update_1"/>
   </protectedRanges>
   <conditionalFormatting sqref="A106:A108 H11:H55 D54:D68 C11:F55 A96 C98:H98 C100:H100 C102:H110 H57:H88 C57:F88 G6:G88 C89:H94 C96:H96">
-    <cfRule type="expression" dxfId="94" priority="158">
+    <cfRule type="expression" dxfId="122" priority="203">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A106:A108 H11:H55 D54:D68 C11:F55 A96 C98:H98 C100:H100 C102:H110 H57:H88 C57:F88 G6:G88 C89:H94 C96:H96">
-    <cfRule type="expression" dxfId="93" priority="157">
+    <cfRule type="expression" dxfId="121" priority="202">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A106:A108 A96 C98:H98 C100:H100 C102:H110 C6:H94 C96:H96 C5:F5 H5">
-    <cfRule type="expression" dxfId="92" priority="156">
+  <conditionalFormatting sqref="A106:A108 A96 C98:H98 C100:H100 C102:H110 C6:H94 C96:H96 C5:F5 H5 N98 N100 N102:N110 N96 N5:N94">
+    <cfRule type="expression" dxfId="120" priority="201">
       <formula>SEARCH("disposal", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C9">
-    <cfRule type="expression" dxfId="91" priority="153">
+    <cfRule type="expression" dxfId="119" priority="198">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C9">
-    <cfRule type="expression" dxfId="90" priority="152">
+    <cfRule type="expression" dxfId="118" priority="197">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="89" priority="151">
+    <cfRule type="expression" dxfId="117" priority="196">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="88" priority="150">
+    <cfRule type="expression" dxfId="116" priority="195">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="87" priority="149">
+    <cfRule type="expression" dxfId="115" priority="194">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="86" priority="148">
+    <cfRule type="expression" dxfId="114" priority="193">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="85" priority="147">
+    <cfRule type="expression" dxfId="113" priority="192">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="84" priority="146">
+    <cfRule type="expression" dxfId="112" priority="191">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="expression" dxfId="83" priority="142">
+    <cfRule type="expression" dxfId="111" priority="187">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D9">
-    <cfRule type="expression" dxfId="82" priority="141">
+    <cfRule type="expression" dxfId="110" priority="186">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="81" priority="140">
+    <cfRule type="expression" dxfId="109" priority="185">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:D56">
-    <cfRule type="expression" dxfId="80" priority="139">
+    <cfRule type="expression" dxfId="108" priority="184">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="79" priority="138">
+    <cfRule type="expression" dxfId="107" priority="183">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="78" priority="137">
+    <cfRule type="expression" dxfId="106" priority="182">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="77" priority="136">
+    <cfRule type="expression" dxfId="105" priority="181">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="76" priority="135">
+    <cfRule type="expression" dxfId="104" priority="180">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E9">
-    <cfRule type="expression" dxfId="75" priority="131">
+    <cfRule type="expression" dxfId="103" priority="176">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E9">
-    <cfRule type="expression" dxfId="74" priority="130">
+    <cfRule type="expression" dxfId="102" priority="175">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="73" priority="129">
+    <cfRule type="expression" dxfId="101" priority="174">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="72" priority="128">
+    <cfRule type="expression" dxfId="100" priority="173">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="71" priority="127">
+    <cfRule type="expression" dxfId="99" priority="172">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="70" priority="126">
+    <cfRule type="expression" dxfId="98" priority="171">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="69" priority="125">
+    <cfRule type="expression" dxfId="97" priority="170">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="68" priority="124">
+    <cfRule type="expression" dxfId="96" priority="169">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F9">
-    <cfRule type="expression" dxfId="67" priority="120">
+    <cfRule type="expression" dxfId="95" priority="165">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F9">
-    <cfRule type="expression" dxfId="66" priority="119">
+    <cfRule type="expression" dxfId="94" priority="164">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="65" priority="118">
+    <cfRule type="expression" dxfId="93" priority="163">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="64" priority="117">
+    <cfRule type="expression" dxfId="92" priority="162">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="63" priority="116">
+    <cfRule type="expression" dxfId="91" priority="161">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="62" priority="115">
+    <cfRule type="expression" dxfId="90" priority="160">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="expression" dxfId="61" priority="107">
+    <cfRule type="expression" dxfId="89" priority="152">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="expression" dxfId="60" priority="106">
+    <cfRule type="expression" dxfId="88" priority="151">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="59" priority="105">
+    <cfRule type="expression" dxfId="87" priority="150">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="58" priority="104">
+    <cfRule type="expression" dxfId="86" priority="149">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="57" priority="100">
+    <cfRule type="expression" dxfId="85" priority="145">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="56" priority="99">
+    <cfRule type="expression" dxfId="84" priority="144">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="expression" dxfId="55" priority="98">
+    <cfRule type="expression" dxfId="83" priority="143">
       <formula>SEARCH("breakdown", $K58)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58">
-    <cfRule type="expression" dxfId="54" priority="97">
+    <cfRule type="expression" dxfId="82" priority="142">
       <formula>SEARCH("issues", $K58)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="53" priority="96">
+    <cfRule type="expression" dxfId="81" priority="141">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="52" priority="95">
+    <cfRule type="expression" dxfId="80" priority="140">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="expression" dxfId="51" priority="94">
+    <cfRule type="expression" dxfId="79" priority="139">
       <formula>SEARCH("breakdown", $K57)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="expression" dxfId="50" priority="93">
+    <cfRule type="expression" dxfId="78" priority="138">
       <formula>SEARCH("issues", $K57)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H9">
-    <cfRule type="expression" dxfId="49" priority="90">
+    <cfRule type="expression" dxfId="77" priority="135">
       <formula>SEARCH("breakdown", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H9">
-    <cfRule type="expression" dxfId="48" priority="89">
+    <cfRule type="expression" dxfId="76" priority="134">
       <formula>SEARCH("issues", $K6)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="expression" dxfId="47" priority="88">
+    <cfRule type="expression" dxfId="75" priority="133">
       <formula>SEARCH("breakdown", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="expression" dxfId="46" priority="87">
+    <cfRule type="expression" dxfId="74" priority="132">
       <formula>SEARCH("issues", $K56)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="45" priority="86">
+    <cfRule type="expression" dxfId="73" priority="131">
       <formula>SEARCH("breakdown", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="44" priority="85">
+    <cfRule type="expression" dxfId="72" priority="130">
       <formula>SEARCH("issues", $K10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="43" priority="84">
+    <cfRule type="expression" dxfId="71" priority="129">
       <formula>SEARCH("breakdown", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="42" priority="83">
+    <cfRule type="expression" dxfId="70" priority="128">
       <formula>SEARCH("issues", $K5)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="expression" dxfId="41" priority="78">
+    <cfRule type="expression" dxfId="69" priority="123">
       <formula>SEARCH("breakdown", $K69)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="expression" dxfId="40" priority="77">
+    <cfRule type="expression" dxfId="68" priority="122">
       <formula>SEARCH("issues", $K69)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="39" priority="76">
+    <cfRule type="expression" dxfId="67" priority="121">
       <formula>SEARCH("breakdown", $K70)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="38" priority="75">
+    <cfRule type="expression" dxfId="66" priority="120">
       <formula>SEARCH("issues", $K70)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="37" priority="74">
+    <cfRule type="expression" dxfId="65" priority="119">
       <formula>SEARCH("breakdown", $K74)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="36" priority="73">
+    <cfRule type="expression" dxfId="64" priority="118">
       <formula>SEARCH("issues", $K74)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="35" priority="72">
+    <cfRule type="expression" dxfId="63" priority="117">
       <formula>SEARCH("breakdown", $K75)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="34" priority="71">
+    <cfRule type="expression" dxfId="62" priority="116">
       <formula>SEARCH("issues", $K75)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="33" priority="70">
+    <cfRule type="expression" dxfId="61" priority="115">
       <formula>SEARCH("breakdown", $K76)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="32" priority="69">
+    <cfRule type="expression" dxfId="60" priority="114">
       <formula>SEARCH("issues", $K76)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="31" priority="68">
+    <cfRule type="expression" dxfId="59" priority="113">
       <formula>SEARCH("breakdown", $K77)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="30" priority="67">
+    <cfRule type="expression" dxfId="58" priority="112">
       <formula>SEARCH("issues", $K77)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="29" priority="66">
+    <cfRule type="expression" dxfId="57" priority="111">
       <formula>SEARCH("breakdown", $K7)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="28" priority="65">
+    <cfRule type="expression" dxfId="56" priority="110">
       <formula>SEARCH("issues", $K7)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="27" priority="64">
+    <cfRule type="expression" dxfId="55" priority="109">
       <formula>SEARCH("breakdown", $K11)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="26" priority="63">
+    <cfRule type="expression" dxfId="54" priority="108">
       <formula>SEARCH("issues", $K11)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="25" priority="62">
+    <cfRule type="expression" dxfId="53" priority="107">
       <formula>SEARCH("breakdown", $K104)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="expression" dxfId="24" priority="61">
+    <cfRule type="expression" dxfId="52" priority="106">
       <formula>SEARCH("issues", $K104)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="23" priority="60">
+    <cfRule type="expression" dxfId="51" priority="105">
       <formula>SEARCH("breakdown", $K105)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105">
-    <cfRule type="expression" dxfId="22" priority="59">
+    <cfRule type="expression" dxfId="50" priority="104">
       <formula>SEARCH("issues", $K105)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="21" priority="58">
+    <cfRule type="expression" dxfId="49" priority="103">
       <formula>SEARCH("breakdown", $K106)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="20" priority="57">
+    <cfRule type="expression" dxfId="48" priority="102">
       <formula>SEARCH("issues", $K106)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="19" priority="56">
+    <cfRule type="expression" dxfId="47" priority="101">
       <formula>SEARCH("breakdown", $K107)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107">
-    <cfRule type="expression" dxfId="18" priority="55">
+    <cfRule type="expression" dxfId="46" priority="100">
       <formula>SEARCH("issues", $K107)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="17" priority="42">
+    <cfRule type="expression" dxfId="45" priority="87">
       <formula>SEARCH("breakdown", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="16" priority="41">
+    <cfRule type="expression" dxfId="44" priority="86">
       <formula>SEARCH("issues", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97 C97:H97">
-    <cfRule type="expression" dxfId="15" priority="40">
+    <cfRule type="expression" dxfId="43" priority="85">
       <formula>SEARCH("disposal", $K97)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="14" priority="39">
+    <cfRule type="expression" dxfId="42" priority="84">
       <formula>SEARCH("breakdown", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="13" priority="38">
+    <cfRule type="expression" dxfId="41" priority="83">
       <formula>SEARCH("issues", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:H99">
-    <cfRule type="expression" dxfId="12" priority="37">
+    <cfRule type="expression" dxfId="40" priority="82">
       <formula>SEARCH("disposal", $K99)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="11" priority="36">
+    <cfRule type="expression" dxfId="39" priority="81">
       <formula>SEARCH("breakdown", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="10" priority="35">
+    <cfRule type="expression" dxfId="38" priority="80">
       <formula>SEARCH("issues", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:H101">
-    <cfRule type="expression" dxfId="9" priority="34">
+    <cfRule type="expression" dxfId="37" priority="79">
       <formula>SEARCH("disposal", $K101)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="8" priority="33">
+    <cfRule type="expression" dxfId="36" priority="78">
       <formula>SEARCH("breakdown", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="7" priority="32">
+    <cfRule type="expression" dxfId="35" priority="77">
       <formula>SEARCH("issues", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:H95">
-    <cfRule type="expression" dxfId="6" priority="31">
+    <cfRule type="expression" dxfId="34" priority="76">
       <formula>SEARCH("disposal", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="5" priority="30">
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="33" priority="75">
       <formula>SEARCH("major issues", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="4" priority="28" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="32" priority="73" stopIfTrue="1">
       <formula>SEARCH("disposal", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B26 B28:B1048576">
-    <cfRule type="expression" dxfId="3" priority="29">
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="expression" dxfId="31" priority="74">
       <formula>SEARCH("breakdown", $J2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="2" priority="24">
-      <formula>SEARCH("major issues", $J2)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="1" priority="22" stopIfTrue="1">
-      <formula>SEARCH("disposal", $J2)&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="0" priority="23">
-      <formula>SEARCH("breakdown", $J2)&gt;0</formula>
+  <conditionalFormatting sqref="N11:N55 N98 N100 N102:N110 N57:N94 N96">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>SEARCH("breakdown", $K11)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:N55 N98 N100 N102:N110 N57:N94 N96">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>SEARCH("issues", $K11)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:N9">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>SEARCH("breakdown", $K6)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:N9">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>SEARCH("issues", $K6)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N56">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>SEARCH("breakdown", $K56)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N56">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>SEARCH("issues", $K56)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>SEARCH("breakdown", $K10)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>SEARCH("issues", $K10)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>SEARCH("breakdown", $K5)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>SEARCH("issues", $K5)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N97">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>SEARCH("breakdown", $K97)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N97">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>SEARCH("issues", $K97)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N97">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>SEARCH("disposal", $K97)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N99">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>SEARCH("breakdown", $K99)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N99">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>SEARCH("issues", $K99)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N99">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>SEARCH("disposal", $K99)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N101">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>SEARCH("breakdown", $K101)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N101">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>SEARCH("issues", $K101)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N101">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>SEARCH("disposal", $K101)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N95">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>SEARCH("breakdown", $K95)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N95">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>SEARCH("issues", $K95)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N95">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>SEARCH("disposal", $K95)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>